<commit_message>
Se creo en pdf estudio de permisos y roles final 3.0
</commit_message>
<xml_diff>
--- a/Estudio de Roles y Seguridad 3.0.xlsx
+++ b/Estudio de Roles y Seguridad 3.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESI 2020\Doc Proyecto\Tercer Entrega\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESI 2020\Doc Proyecto\Tercer Entrega\Base de datos\BaseDeDatos_CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -137,10 +137,10 @@
     <t>dbTriage</t>
   </si>
   <si>
-    <t>192.168.3.%</t>
-  </si>
-  <si>
     <t>Setting</t>
+  </si>
+  <si>
+    <t>192.168.1.%</t>
   </si>
 </sst>
 </file>
@@ -525,6 +525,9 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,9 +541,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -877,8 +877,8 @@
   </sheetPr>
   <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="P54" sqref="P54"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="I80" sqref="I80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
@@ -911,11 +911,11 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -943,11 +943,11 @@
       <c r="A4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="20" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1324,36 +1324,36 @@
       <c r="L21" s="23"/>
     </row>
     <row r="22" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
     </row>
     <row r="23" spans="1:12" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="35"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="36"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
@@ -1408,7 +1408,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="14"/>
@@ -1428,7 +1428,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="15"/>
@@ -1446,7 +1446,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="14"/>
@@ -1466,7 +1466,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="15"/>
@@ -1486,7 +1486,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="14"/>
@@ -1506,7 +1506,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="15"/>
@@ -1528,7 +1528,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="14"/>
@@ -1548,7 +1548,7 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="15"/>
@@ -1566,7 +1566,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="14"/>
@@ -1590,7 +1590,7 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="15"/>
@@ -1608,7 +1608,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="14"/>
@@ -1628,7 +1628,7 @@
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="15"/>
@@ -1648,7 +1648,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="14"/>
@@ -1666,14 +1666,14 @@
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K38" s="17"/>
       <c r="L38" s="18"/>
     </row>
     <row r="39" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1685,8 +1685,8 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="17" t="s">
-        <v>37</v>
+      <c r="J39" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="K39" s="17"/>
       <c r="L39" s="18"/>
@@ -1704,42 +1704,42 @@
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>
       <c r="J40" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K40" s="22"/>
       <c r="L40" s="23"/>
     </row>
     <row r="41" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
     </row>
     <row r="42" spans="1:12" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="38" t="s">
+      <c r="B42" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="36"/>
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
@@ -1798,7 +1798,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="14"/>
@@ -1824,7 +1824,7 @@
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K45" s="4"/>
       <c r="L45" s="15"/>
@@ -1848,7 +1848,7 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="14"/>
@@ -1872,7 +1872,7 @@
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K47" s="4"/>
       <c r="L47" s="15"/>
@@ -1896,7 +1896,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="14"/>
@@ -1922,7 +1922,7 @@
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K49" s="4"/>
       <c r="L49" s="15"/>
@@ -1940,7 +1940,7 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K50" s="3"/>
       <c r="L50" s="14"/>
@@ -1964,7 +1964,7 @@
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="15"/>
@@ -1988,7 +1988,7 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K52" s="3"/>
       <c r="L52" s="14"/>
@@ -2008,7 +2008,7 @@
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="15"/>
@@ -2026,7 +2026,7 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K54" s="3"/>
       <c r="L54" s="14"/>
@@ -2044,7 +2044,7 @@
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K55" s="4"/>
       <c r="L55" s="15"/>
@@ -2062,7 +2062,7 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K56" s="3"/>
       <c r="L56" s="14"/>
@@ -2088,14 +2088,14 @@
       <c r="H57" s="17"/>
       <c r="I57" s="17"/>
       <c r="J57" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K57" s="17"/>
       <c r="L57" s="18"/>
     </row>
     <row r="58" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2111,8 +2111,8 @@
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
-      <c r="J58" s="17" t="s">
-        <v>37</v>
+      <c r="J58" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="K58" s="17"/>
       <c r="L58" s="18"/>
@@ -2132,7 +2132,7 @@
       </c>
       <c r="I59" s="17"/>
       <c r="J59" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K59" s="22" t="s">
         <v>27</v>
@@ -2145,9 +2145,9 @@
       <c r="A60" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
       <c r="E60" s="31"/>
       <c r="F60" s="31"/>
       <c r="G60" s="31"/>
@@ -2413,15 +2413,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B42:D42"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="J42:L42"/>
     <mergeCell ref="E23:L23"/>
     <mergeCell ref="A22:L22"/>
     <mergeCell ref="A41:L41"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B42:D42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>